<commit_message>
elaborate on the concept `Project` in Blik
</commit_message>
<xml_diff>
--- a/Blik/projecten.xlsx
+++ b/Blik/projecten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="10584"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="Projecten" sheetId="1" r:id="rId1"/>
@@ -16,26 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
   <si>
     <t>projectnaam</t>
   </si>
   <si>
-    <t>Omschrijving project</t>
-  </si>
-  <si>
-    <t>Bijdrage aan resultaat:</t>
-  </si>
-  <si>
-    <t>Bijdrage aan C&amp;V Verbeterplan</t>
-  </si>
-  <si>
-    <t>Wie:</t>
-  </si>
-  <si>
-    <t>Wanneer:</t>
-  </si>
-  <si>
     <t>Klachten rookvrije werkplek</t>
   </si>
   <si>
@@ -202,9 +187,6 @@
   </si>
   <si>
     <t>C&amp;V horecateams (waar mogelijk gekoppeld aan de formule-aanpakinspecties)</t>
-  </si>
-  <si>
-    <t>nader te bepalen</t>
   </si>
   <si>
     <t>Corinne Schouten</t>
@@ -425,13 +407,28 @@
   </si>
   <si>
     <t>[Persoon/]</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>verbetering</t>
+  </si>
+  <si>
+    <t>resultaat</t>
+  </si>
+  <si>
+    <t>eenheid</t>
+  </si>
+  <si>
+    <t>wanneer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,11 +468,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -549,6 +551,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -583,6 +586,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -758,743 +762,741 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="43.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>133</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="28.8">
+    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="72">
-      <c r="A4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="57.6">
+    <row r="5" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="43.2">
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="43.2">
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="43.2">
+    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="28.8">
+    <row r="9" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K9" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="43.2">
+    <row r="10" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="172.8">
+    <row r="11" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="43.2">
+    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="172.8">
+    <row r="13" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="72">
+    <row r="14" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="K14" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1506,24 +1508,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>